<commit_message>
Rearranged main.py, added dundermain and removed some redundant code. Reworked the spreadsheets and extended the readme
</commit_message>
<xml_diff>
--- a/Final/Lesson Plans/Subject 1.xlsx
+++ b/Final/Lesson Plans/Subject 1.xlsx
@@ -1,58 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26306"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb87c8faced79414/Desktop/Test Lesson/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC10489F79D95CFA5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA6B4C7E-105A-4548-873E-800A04D2D3F9}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="11_F25DC773A252ABDACC10489F79D95CFA5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{045F0A1D-A056-4214-B586-470FA0EF4C0F}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Do a thing</t>
-  </si>
-  <si>
-    <t>Do another thing</t>
-  </si>
-  <si>
-    <t>Do a third thing</t>
-  </si>
-  <si>
-    <t>Lorem impusm</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>This is Lesson 0. If you don't want a lesson 0, fair enough! Just start in row 2</t>
+  </si>
+  <si>
+    <t>This is Lesson 1. Lesson 1 should be in row 2 etc.</t>
+  </si>
+  <si>
+    <t>If your lessons are over here, set Column Number to 1 in lesson_indexes.json. If they are in another column, set the appropriate column number</t>
+  </si>
+  <si>
+    <t>Lesson 2</t>
+  </si>
+  <si>
+    <t>Lesson 3</t>
+  </si>
+  <si>
+    <t>Lesson 4</t>
+  </si>
+  <si>
+    <t>You get the idea</t>
+  </si>
+  <si>
+    <t>Lorum Impusm</t>
   </si>
   <si>
     <t>Dolor sit amet</t>
-  </si>
-  <si>
-    <t>Im bored</t>
-  </si>
-  <si>
-    <t>Lesson Plan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,8 +98,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -98,10 +121,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -367,51 +386,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" customWidth="1"/>
+    <col min="1" max="1" width="47.140625" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:2" ht="30.75">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="43.5" customHeight="1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>5</v>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>